<commit_message>
Update external data 1
Data updated in order of do-file use
</commit_message>
<xml_diff>
--- a/data-input/wb-data/global-economic-monitor/GDP Deflator at Market Prices, LCU.xlsx
+++ b/data-input/wb-data/global-economic-monitor/GDP Deflator at Market Prices, LCU.xlsx
@@ -5,7 +5,7 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="quarterly" sheetId="1" r:id="R89fb6e80402f4b02"/>
+    <sheet name="quarterly" sheetId="1" r:id="Rb0a6ddfb6ed64081"/>
   </sheets>
 </workbook>
 </file>
@@ -1259,7 +1259,7 @@
         <v>0.729814</v>
       </c>
       <c r="AD3" s="0">
-        <v>0.747505</v>
+        <v>0.747428</v>
       </c>
       <c r="AE3" s="0">
         <v>0.619337</v>
@@ -1522,7 +1522,7 @@
         <v>0.730914</v>
       </c>
       <c r="AD4" s="0">
-        <v>0.752136</v>
+        <v>0.752161</v>
       </c>
       <c r="AE4" s="0">
         <v>0.626918</v>
@@ -1785,7 +1785,7 @@
         <v>0.733286</v>
       </c>
       <c r="AD5" s="0">
-        <v>0.756523</v>
+        <v>0.756437</v>
       </c>
       <c r="AE5" s="0">
         <v>0.634485</v>
@@ -2048,7 +2048,7 @@
         <v>0.736155</v>
       </c>
       <c r="AD6" s="0">
-        <v>0.759396</v>
+        <v>0.759803</v>
       </c>
       <c r="AE6" s="0">
         <v>0.641428</v>
@@ -2311,7 +2311,7 @@
         <v>0.735767</v>
       </c>
       <c r="AD7" s="0">
-        <v>0.765688</v>
+        <v>0.765523</v>
       </c>
       <c r="AE7" s="0">
         <v>0.64784</v>
@@ -2574,7 +2574,7 @@
         <v>0.736118</v>
       </c>
       <c r="AD8" s="0">
-        <v>0.767869</v>
+        <v>0.767858</v>
       </c>
       <c r="AE8" s="0">
         <v>0.649126</v>
@@ -2837,7 +2837,7 @@
         <v>0.739768</v>
       </c>
       <c r="AD9" s="0">
-        <v>0.771512</v>
+        <v>0.771461</v>
       </c>
       <c r="AE9" s="0">
         <v>0.646936</v>
@@ -3100,7 +3100,7 @@
         <v>0.745731</v>
       </c>
       <c r="AD10" s="0">
-        <v>0.772529</v>
+        <v>0.772519</v>
       </c>
       <c r="AE10" s="0">
         <v>0.653422</v>
@@ -3363,7 +3363,7 @@
         <v>0.750097</v>
       </c>
       <c r="AD11" s="0">
-        <v>0.779614</v>
+        <v>0.779579</v>
       </c>
       <c r="AE11" s="0">
         <v>0.663554</v>
@@ -3504,7 +3504,7 @@
         <v>88</v>
       </c>
       <c r="BY11" s="0">
-        <v>0.683263</v>
+        <v>0.673732</v>
       </c>
       <c r="BZ11" s="0">
         <v>0.730698</v>
@@ -3626,7 +3626,7 @@
         <v>0.753698</v>
       </c>
       <c r="AD12" s="0">
-        <v>0.781269</v>
+        <v>0.781566</v>
       </c>
       <c r="AE12" s="0">
         <v>0.6607</v>
@@ -3767,7 +3767,7 @@
         <v>88</v>
       </c>
       <c r="BY12" s="0">
-        <v>0.682889</v>
+        <v>0.673299</v>
       </c>
       <c r="BZ12" s="0">
         <v>0.752124</v>
@@ -3889,7 +3889,7 @@
         <v>0.751188</v>
       </c>
       <c r="AD13" s="0">
-        <v>0.782552</v>
+        <v>0.782526</v>
       </c>
       <c r="AE13" s="0">
         <v>0.667596</v>
@@ -4030,7 +4030,7 @@
         <v>88</v>
       </c>
       <c r="BY13" s="0">
-        <v>0.688449</v>
+        <v>0.678777</v>
       </c>
       <c r="BZ13" s="0">
         <v>0.76191</v>
@@ -4152,7 +4152,7 @@
         <v>0.755566</v>
       </c>
       <c r="AD14" s="0">
-        <v>0.783229</v>
+        <v>0.783441</v>
       </c>
       <c r="AE14" s="0">
         <v>0.671825</v>
@@ -4293,7 +4293,7 @@
         <v>88</v>
       </c>
       <c r="BY14" s="0">
-        <v>0.697076</v>
+        <v>0.687294</v>
       </c>
       <c r="BZ14" s="0">
         <v>0.762186</v>
@@ -4415,7 +4415,7 @@
         <v>0.754736</v>
       </c>
       <c r="AD15" s="0">
-        <v>0.785733</v>
+        <v>0.785902</v>
       </c>
       <c r="AE15" s="0">
         <v>0.672796</v>
@@ -4556,7 +4556,7 @@
         <v>88</v>
       </c>
       <c r="BY15" s="0">
-        <v>0.700423</v>
+        <v>0.690631</v>
       </c>
       <c r="BZ15" s="0">
         <v>0.76782</v>
@@ -4678,7 +4678,7 @@
         <v>0.763122</v>
       </c>
       <c r="AD16" s="0">
-        <v>0.788045</v>
+        <v>0.787905</v>
       </c>
       <c r="AE16" s="0">
         <v>0.670582</v>
@@ -4819,7 +4819,7 @@
         <v>88</v>
       </c>
       <c r="BY16" s="0">
-        <v>0.704139</v>
+        <v>0.694253</v>
       </c>
       <c r="BZ16" s="0">
         <v>0.778605</v>
@@ -4941,7 +4941,7 @@
         <v>0.769388</v>
       </c>
       <c r="AD17" s="0">
-        <v>0.789139</v>
+        <v>0.78897</v>
       </c>
       <c r="AE17" s="0">
         <v>0.670545</v>
@@ -5082,7 +5082,7 @@
         <v>88</v>
       </c>
       <c r="BY17" s="0">
-        <v>0.706229</v>
+        <v>0.69631</v>
       </c>
       <c r="BZ17" s="0">
         <v>0.791614</v>
@@ -5204,7 +5204,7 @@
         <v>0.778215</v>
       </c>
       <c r="AD18" s="0">
-        <v>0.792987</v>
+        <v>0.792905</v>
       </c>
       <c r="AE18" s="0">
         <v>0.680796</v>
@@ -5345,7 +5345,7 @@
         <v>88</v>
       </c>
       <c r="BY18" s="0">
-        <v>0.712559</v>
+        <v>0.702546</v>
       </c>
       <c r="BZ18" s="0">
         <v>0.809563</v>
@@ -5467,7 +5467,7 @@
         <v>0.791117</v>
       </c>
       <c r="AD19" s="0">
-        <v>0.793612</v>
+        <v>0.793231</v>
       </c>
       <c r="AE19" s="0">
         <v>0.681133</v>
@@ -5608,7 +5608,7 @@
         <v>0.448459</v>
       </c>
       <c r="BY19" s="0">
-        <v>0.724098</v>
+        <v>0.713949</v>
       </c>
       <c r="BZ19" s="0">
         <v>0.826323</v>
@@ -5730,7 +5730,7 @@
         <v>0.798565</v>
       </c>
       <c r="AD20" s="0">
-        <v>0.796446</v>
+        <v>0.796236</v>
       </c>
       <c r="AE20" s="0">
         <v>0.68673</v>
@@ -5871,7 +5871,7 @@
         <v>0.457341</v>
       </c>
       <c r="BY20" s="0">
-        <v>0.732481</v>
+        <v>0.722227</v>
       </c>
       <c r="BZ20" s="0">
         <v>0.826303</v>
@@ -5993,7 +5993,7 @@
         <v>0.800303</v>
       </c>
       <c r="AD21" s="0">
-        <v>0.800046</v>
+        <v>0.799851</v>
       </c>
       <c r="AE21" s="0">
         <v>0.692097</v>
@@ -6134,7 +6134,7 @@
         <v>0.470184</v>
       </c>
       <c r="BY21" s="0">
-        <v>0.736133</v>
+        <v>0.725834</v>
       </c>
       <c r="BZ21" s="0">
         <v>0.836219</v>
@@ -6256,7 +6256,7 @@
         <v>0.80451</v>
       </c>
       <c r="AD22" s="0">
-        <v>0.801979</v>
+        <v>0.802495</v>
       </c>
       <c r="AE22" s="0">
         <v>0.699239</v>
@@ -6397,7 +6397,7 @@
         <v>0.485094</v>
       </c>
       <c r="BY22" s="0">
-        <v>0.736223</v>
+        <v>0.725893</v>
       </c>
       <c r="BZ22" s="0">
         <v>0.839588</v>
@@ -6519,7 +6519,7 @@
         <v>0.794218</v>
       </c>
       <c r="AD23" s="0">
-        <v>0.806664</v>
+        <v>0.806563</v>
       </c>
       <c r="AE23" s="0">
         <v>0.707091</v>
@@ -6660,7 +6660,7 @@
         <v>0.49774</v>
       </c>
       <c r="BY23" s="0">
-        <v>0.740992</v>
+        <v>0.730594</v>
       </c>
       <c r="BZ23" s="0">
         <v>0.853962</v>
@@ -6782,7 +6782,7 @@
         <v>0.797133</v>
       </c>
       <c r="AD24" s="0">
-        <v>0.808623</v>
+        <v>0.808474</v>
       </c>
       <c r="AE24" s="0">
         <v>0.719103</v>
@@ -6923,7 +6923,7 @@
         <v>0.512828</v>
       </c>
       <c r="BY24" s="0">
-        <v>0.73545</v>
+        <v>0.725162</v>
       </c>
       <c r="BZ24" s="0">
         <v>0.864836</v>
@@ -7045,7 +7045,7 @@
         <v>0.797376</v>
       </c>
       <c r="AD25" s="0">
-        <v>0.809588</v>
+        <v>0.809582</v>
       </c>
       <c r="AE25" s="0">
         <v>0.722503</v>
@@ -7186,7 +7186,7 @@
         <v>0.526277</v>
       </c>
       <c r="BY25" s="0">
-        <v>0.745506</v>
+        <v>0.735062</v>
       </c>
       <c r="BZ25" s="0">
         <v>0.870952</v>
@@ -7308,7 +7308,7 @@
         <v>0.802659</v>
       </c>
       <c r="AD26" s="0">
-        <v>0.810137</v>
+        <v>0.810636</v>
       </c>
       <c r="AE26" s="0">
         <v>0.722941</v>
@@ -7449,7 +7449,7 @@
         <v>0.533037</v>
       </c>
       <c r="BY26" s="0">
-        <v>0.737653</v>
+        <v>0.727328</v>
       </c>
       <c r="BZ26" s="0">
         <v>0.874451</v>
@@ -7571,7 +7571,7 @@
         <v>0.803801</v>
       </c>
       <c r="AD27" s="0">
-        <v>0.812654</v>
+        <v>0.812578</v>
       </c>
       <c r="AE27" s="0">
         <v>0.727087</v>
@@ -7712,7 +7712,7 @@
         <v>0.545741</v>
       </c>
       <c r="BY27" s="0">
-        <v>0.74473</v>
+        <v>0.73437</v>
       </c>
       <c r="BZ27" s="0">
         <v>0.87826</v>
@@ -7834,7 +7834,7 @@
         <v>0.81338</v>
       </c>
       <c r="AD28" s="0">
-        <v>0.814861</v>
+        <v>0.814743</v>
       </c>
       <c r="AE28" s="0">
         <v>0.728138</v>
@@ -7975,7 +7975,7 @@
         <v>0.555738</v>
       </c>
       <c r="BY28" s="0">
-        <v>0.750555</v>
+        <v>0.74001</v>
       </c>
       <c r="BZ28" s="0">
         <v>0.887395</v>
@@ -8097,7 +8097,7 @@
         <v>0.818033</v>
       </c>
       <c r="AD29" s="0">
-        <v>0.81719</v>
+        <v>0.817053</v>
       </c>
       <c r="AE29" s="0">
         <v>0.742104</v>
@@ -8238,7 +8238,7 @@
         <v>0.564567</v>
       </c>
       <c r="BY29" s="0">
-        <v>0.751094</v>
+        <v>0.740575</v>
       </c>
       <c r="BZ29" s="0">
         <v>0.910627</v>
@@ -8360,7 +8360,7 @@
         <v>0.823354</v>
       </c>
       <c r="AD30" s="0">
-        <v>0.819308</v>
+        <v>0.819516</v>
       </c>
       <c r="AE30" s="0">
         <v>0.730552</v>
@@ -8501,7 +8501,7 @@
         <v>0.578173</v>
       </c>
       <c r="BY30" s="0">
-        <v>0.75617</v>
+        <v>0.745597</v>
       </c>
       <c r="BZ30" s="0">
         <v>0.941022</v>
@@ -8623,7 +8623,7 @@
         <v>0.837242</v>
       </c>
       <c r="AD31" s="0">
-        <v>0.820894</v>
+        <v>0.820892</v>
       </c>
       <c r="AE31" s="0">
         <v>0.736597</v>
@@ -8764,7 +8764,7 @@
         <v>0.58599</v>
       </c>
       <c r="BY31" s="0">
-        <v>0.755436</v>
+        <v>0.744863</v>
       </c>
       <c r="BZ31" s="0">
         <v>0.994841</v>
@@ -8886,7 +8886,7 @@
         <v>0.840036</v>
       </c>
       <c r="AD32" s="0">
-        <v>0.825101</v>
+        <v>0.825388</v>
       </c>
       <c r="AE32" s="0">
         <v>0.737262</v>
@@ -9027,7 +9027,7 @@
         <v>0.596107</v>
       </c>
       <c r="BY32" s="0">
-        <v>0.755935</v>
+        <v>0.745368</v>
       </c>
       <c r="BZ32" s="0">
         <v>0.984965</v>
@@ -9149,7 +9149,7 @@
         <v>0.842153</v>
       </c>
       <c r="AD33" s="0">
-        <v>0.824836</v>
+        <v>0.824938</v>
       </c>
       <c r="AE33" s="0">
         <v>0.737952</v>
@@ -9290,7 +9290,7 @@
         <v>0.607307</v>
       </c>
       <c r="BY33" s="0">
-        <v>0.755167</v>
+        <v>0.744581</v>
       </c>
       <c r="BZ33" s="0">
         <v>0.973357</v>
@@ -9412,7 +9412,7 @@
         <v>0.841011</v>
       </c>
       <c r="AD34" s="0">
-        <v>0.824265</v>
+        <v>0.824546</v>
       </c>
       <c r="AE34" s="0">
         <v>0.750725</v>
@@ -9553,7 +9553,7 @@
         <v>0.618887</v>
       </c>
       <c r="BY34" s="0">
-        <v>0.760548</v>
+        <v>0.749899</v>
       </c>
       <c r="BZ34" s="0">
         <v>0.955345</v>
@@ -9675,7 +9675,7 @@
         <v>0.841043</v>
       </c>
       <c r="AD35" s="0">
-        <v>0.824734</v>
+        <v>0.824928</v>
       </c>
       <c r="AE35" s="0">
         <v>0.751431</v>
@@ -9816,7 +9816,7 @@
         <v>0.631565</v>
       </c>
       <c r="BY35" s="0">
-        <v>0.760228</v>
+        <v>0.749591</v>
       </c>
       <c r="BZ35" s="0">
         <v>0.956313</v>
@@ -9938,7 +9938,7 @@
         <v>0.84548</v>
       </c>
       <c r="AD36" s="0">
-        <v>0.825295</v>
+        <v>0.825666</v>
       </c>
       <c r="AE36" s="0">
         <v>0.747466</v>
@@ -10079,7 +10079,7 @@
         <v>0.62742</v>
       </c>
       <c r="BY36" s="0">
-        <v>0.762393</v>
+        <v>0.751702</v>
       </c>
       <c r="BZ36" s="0">
         <v>0.949568</v>
@@ -10201,7 +10201,7 @@
         <v>0.850818</v>
       </c>
       <c r="AD37" s="0">
-        <v>0.825809</v>
+        <v>0.825869</v>
       </c>
       <c r="AE37" s="0">
         <v>0.743914</v>
@@ -10342,7 +10342,7 @@
         <v>0.648276</v>
       </c>
       <c r="BY37" s="0">
-        <v>0.764951</v>
+        <v>0.754217</v>
       </c>
       <c r="BZ37" s="0">
         <v>0.947418</v>
@@ -10464,7 +10464,7 @@
         <v>0.854878</v>
       </c>
       <c r="AD38" s="0">
-        <v>0.826769</v>
+        <v>0.826492</v>
       </c>
       <c r="AE38" s="0">
         <v>0.745501</v>
@@ -10605,7 +10605,7 @@
         <v>0.657736</v>
       </c>
       <c r="BY38" s="0">
-        <v>0.77011</v>
+        <v>0.759305</v>
       </c>
       <c r="BZ38" s="0">
         <v>0.953873</v>
@@ -10694,7 +10694,7 @@
         <v>0.574524</v>
       </c>
       <c r="S39" s="0">
-        <v>0.701239</v>
+        <v>0.701183</v>
       </c>
       <c r="T39" s="0">
         <v>0.322561</v>
@@ -10727,7 +10727,7 @@
         <v>0.84989</v>
       </c>
       <c r="AD39" s="0">
-        <v>0.832103</v>
+        <v>0.831986</v>
       </c>
       <c r="AE39" s="0">
         <v>0.756409</v>
@@ -10868,7 +10868,7 @@
         <v>0.661481</v>
       </c>
       <c r="BY39" s="0">
-        <v>0.770188</v>
+        <v>0.759367</v>
       </c>
       <c r="BZ39" s="0">
         <v>0.94416</v>
@@ -10990,7 +10990,7 @@
         <v>0.859269</v>
       </c>
       <c r="AD40" s="0">
-        <v>0.836444</v>
+        <v>0.836278</v>
       </c>
       <c r="AE40" s="0">
         <v>0.761275</v>
@@ -11131,7 +11131,7 @@
         <v>0.669004</v>
       </c>
       <c r="BY40" s="0">
-        <v>0.773779</v>
+        <v>0.762959</v>
       </c>
       <c r="BZ40" s="0">
         <v>0.954531</v>
@@ -11220,7 +11220,7 @@
         <v>0.5801</v>
       </c>
       <c r="S41" s="0">
-        <v>0.751393</v>
+        <v>0.751869</v>
       </c>
       <c r="T41" s="0">
         <v>0.339822</v>
@@ -11253,7 +11253,7 @@
         <v>0.865496</v>
       </c>
       <c r="AD41" s="0">
-        <v>0.840526</v>
+        <v>0.840516</v>
       </c>
       <c r="AE41" s="0">
         <v>0.765081</v>
@@ -11394,7 +11394,7 @@
         <v>0.684194</v>
       </c>
       <c r="BY41" s="0">
-        <v>0.778916</v>
+        <v>0.768003</v>
       </c>
       <c r="BZ41" s="0">
         <v>0.971015</v>
@@ -11483,7 +11483,7 @@
         <v>0.584274</v>
       </c>
       <c r="S42" s="0">
-        <v>0.75333</v>
+        <v>0.752909</v>
       </c>
       <c r="T42" s="0">
         <v>0.328221</v>
@@ -11516,7 +11516,7 @@
         <v>0.872746</v>
       </c>
       <c r="AD42" s="0">
-        <v>0.844428</v>
+        <v>0.844642</v>
       </c>
       <c r="AE42" s="0">
         <v>0.76577</v>
@@ -11657,7 +11657,7 @@
         <v>0.699155</v>
       </c>
       <c r="BY42" s="0">
-        <v>0.781222</v>
+        <v>0.77028</v>
       </c>
       <c r="BZ42" s="0">
         <v>0.988294</v>
@@ -11746,7 +11746,7 @@
         <v>0.591182</v>
       </c>
       <c r="S43" s="0">
-        <v>0.760798</v>
+        <v>0.760617</v>
       </c>
       <c r="T43" s="0">
         <v>0.346643</v>
@@ -11779,7 +11779,7 @@
         <v>0.888144</v>
       </c>
       <c r="AD43" s="0">
-        <v>0.84854</v>
+        <v>0.848589</v>
       </c>
       <c r="AE43" s="0">
         <v>0.762572</v>
@@ -11920,7 +11920,7 @@
         <v>0.715881</v>
       </c>
       <c r="BY43" s="0">
-        <v>0.785983</v>
+        <v>0.774945</v>
       </c>
       <c r="BZ43" s="0">
         <v>0.977298</v>
@@ -12009,7 +12009,7 @@
         <v>0.591381</v>
       </c>
       <c r="S44" s="0">
-        <v>0.778481</v>
+        <v>0.778537</v>
       </c>
       <c r="T44" s="0">
         <v>0.357054</v>
@@ -12042,7 +12042,7 @@
         <v>0.890771</v>
       </c>
       <c r="AD44" s="0">
-        <v>0.853148</v>
+        <v>0.852865</v>
       </c>
       <c r="AE44" s="0">
         <v>0.771564</v>
@@ -12183,7 +12183,7 @@
         <v>0.731809</v>
       </c>
       <c r="BY44" s="0">
-        <v>0.798108</v>
+        <v>0.786957</v>
       </c>
       <c r="BZ44" s="0">
         <v>0.98984</v>
@@ -12272,7 +12272,7 @@
         <v>0.59183</v>
       </c>
       <c r="S45" s="0">
-        <v>0.791297</v>
+        <v>0.791668</v>
       </c>
       <c r="T45" s="0">
         <v>0.365249</v>
@@ -12305,7 +12305,7 @@
         <v>0.891419</v>
       </c>
       <c r="AD45" s="0">
-        <v>0.857208</v>
+        <v>0.857036</v>
       </c>
       <c r="AE45" s="0">
         <v>0.769144</v>
@@ -12446,7 +12446,7 @@
         <v>0.745914</v>
       </c>
       <c r="BY45" s="0">
-        <v>0.792972</v>
+        <v>0.781866</v>
       </c>
       <c r="BZ45" s="0">
         <v>0.988075</v>
@@ -12535,7 +12535,7 @@
         <v>0.591311</v>
       </c>
       <c r="S46" s="0">
-        <v>0.789296</v>
+        <v>0.78905</v>
       </c>
       <c r="T46" s="0">
         <v>0.370786</v>
@@ -12568,7 +12568,7 @@
         <v>0.892261</v>
       </c>
       <c r="AD46" s="0">
-        <v>0.86208</v>
+        <v>0.861848</v>
       </c>
       <c r="AE46" s="0">
         <v>0.773364</v>
@@ -12709,7 +12709,7 @@
         <v>0.757167</v>
       </c>
       <c r="BY46" s="0">
-        <v>0.80287</v>
+        <v>0.791648</v>
       </c>
       <c r="BZ46" s="0">
         <v>0.977586</v>
@@ -12798,7 +12798,7 @@
         <v>0.592124</v>
       </c>
       <c r="S47" s="0">
-        <v>0.796028</v>
+        <v>0.795849</v>
       </c>
       <c r="T47" s="0">
         <v>0.375086</v>
@@ -12831,7 +12831,7 @@
         <v>0.895711</v>
       </c>
       <c r="AD47" s="0">
-        <v>0.866782</v>
+        <v>0.866719</v>
       </c>
       <c r="AE47" s="0">
         <v>0.779753</v>
@@ -12972,7 +12972,7 @@
         <v>0.776548</v>
       </c>
       <c r="BY47" s="0">
-        <v>0.803419</v>
+        <v>0.792184</v>
       </c>
       <c r="BZ47" s="0">
         <v>0.995545</v>
@@ -13061,7 +13061,7 @@
         <v>0.59368</v>
       </c>
       <c r="S48" s="0">
-        <v>0.810883</v>
+        <v>0.811043</v>
       </c>
       <c r="T48" s="0">
         <v>0.39292</v>
@@ -13094,7 +13094,7 @@
         <v>0.899792</v>
       </c>
       <c r="AD48" s="0">
-        <v>0.870415</v>
+        <v>0.870149</v>
       </c>
       <c r="AE48" s="0">
         <v>0.78244</v>
@@ -13235,7 +13235,7 @@
         <v>0.787253</v>
       </c>
       <c r="BY48" s="0">
-        <v>0.80707</v>
+        <v>0.795767</v>
       </c>
       <c r="BZ48" s="0">
         <v>0.995904</v>
@@ -13324,7 +13324,7 @@
         <v>0.595381</v>
       </c>
       <c r="S49" s="0">
-        <v>0.844916</v>
+        <v>0.845318</v>
       </c>
       <c r="T49" s="0">
         <v>0.402268</v>
@@ -13357,7 +13357,7 @@
         <v>0.90008</v>
       </c>
       <c r="AD49" s="0">
-        <v>0.874789</v>
+        <v>0.8748</v>
       </c>
       <c r="AE49" s="0">
         <v>0.788546</v>
@@ -13498,7 +13498,7 @@
         <v>0.798292</v>
       </c>
       <c r="BY49" s="0">
-        <v>0.808038</v>
+        <v>0.796707</v>
       </c>
       <c r="BZ49" s="0">
         <v>0.99644</v>
@@ -13587,7 +13587,7 @@
         <v>0.598045</v>
       </c>
       <c r="S50" s="0">
-        <v>0.853609</v>
+        <v>0.853222</v>
       </c>
       <c r="T50" s="0">
         <v>0.411379</v>
@@ -13620,7 +13620,7 @@
         <v>0.901533</v>
       </c>
       <c r="AD50" s="0">
-        <v>0.879549</v>
+        <v>0.879605</v>
       </c>
       <c r="AE50" s="0">
         <v>0.793419</v>
@@ -13761,7 +13761,7 @@
         <v>0.807349</v>
       </c>
       <c r="BY50" s="0">
-        <v>0.812144</v>
+        <v>0.800786</v>
       </c>
       <c r="BZ50" s="0">
         <v>1.01166</v>
@@ -13850,7 +13850,7 @@
         <v>0.604393</v>
       </c>
       <c r="S51" s="0">
-        <v>0.869075</v>
+        <v>0.868903</v>
       </c>
       <c r="T51" s="0">
         <v>0.421923</v>
@@ -13883,7 +13883,7 @@
         <v>0.903539</v>
       </c>
       <c r="AD51" s="0">
-        <v>0.882539</v>
+        <v>0.882492</v>
       </c>
       <c r="AE51" s="0">
         <v>0.799411</v>
@@ -14024,7 +14024,7 @@
         <v>0.819688</v>
       </c>
       <c r="BY51" s="0">
-        <v>0.819741</v>
+        <v>0.80827</v>
       </c>
       <c r="BZ51" s="0">
         <v>1.018592</v>
@@ -14113,7 +14113,7 @@
         <v>0.606799</v>
       </c>
       <c r="S52" s="0">
-        <v>0.87244</v>
+        <v>0.872571</v>
       </c>
       <c r="T52" s="0">
         <v>0.43141</v>
@@ -14146,7 +14146,7 @@
         <v>0.897784</v>
       </c>
       <c r="AD52" s="0">
-        <v>0.887135</v>
+        <v>0.886968</v>
       </c>
       <c r="AE52" s="0">
         <v>0.801583</v>
@@ -14287,7 +14287,7 @@
         <v>0.834045</v>
       </c>
       <c r="BY52" s="0">
-        <v>0.818855</v>
+        <v>0.807416</v>
       </c>
       <c r="BZ52" s="0">
         <v>1.01378</v>
@@ -14376,7 +14376,7 @@
         <v>0.610558</v>
       </c>
       <c r="S53" s="0">
-        <v>0.891103</v>
+        <v>0.891399</v>
       </c>
       <c r="T53" s="0">
         <v>0.44005</v>
@@ -14409,7 +14409,7 @@
         <v>0.900446</v>
       </c>
       <c r="AD53" s="0">
-        <v>0.891515</v>
+        <v>0.891698</v>
       </c>
       <c r="AE53" s="0">
         <v>0.805333</v>
@@ -14550,7 +14550,7 @@
         <v>0.843829</v>
       </c>
       <c r="BY53" s="0">
-        <v>0.823306</v>
+        <v>0.811769</v>
       </c>
       <c r="BZ53" s="0">
         <v>1.021498</v>
@@ -14639,7 +14639,7 @@
         <v>0.618344</v>
       </c>
       <c r="S54" s="0">
-        <v>0.898817</v>
+        <v>0.898563</v>
       </c>
       <c r="T54" s="0">
         <v>0.457394</v>
@@ -14672,7 +14672,7 @@
         <v>0.903107</v>
       </c>
       <c r="AD54" s="0">
-        <v>0.89533</v>
+        <v>0.895521</v>
       </c>
       <c r="AE54" s="0">
         <v>0.813355</v>
@@ -14813,7 +14813,7 @@
         <v>0.84562</v>
       </c>
       <c r="BY54" s="0">
-        <v>0.824531</v>
+        <v>0.813003</v>
       </c>
       <c r="BZ54" s="0">
         <v>1.032522</v>
@@ -14902,7 +14902,7 @@
         <v>0.633087</v>
       </c>
       <c r="S55" s="0">
-        <v>0.918733</v>
+        <v>0.918608</v>
       </c>
       <c r="T55" s="0">
         <v>0.473163</v>
@@ -14935,7 +14935,7 @@
         <v>0.906339</v>
       </c>
       <c r="AD55" s="0">
-        <v>0.899728</v>
+        <v>0.899641</v>
       </c>
       <c r="AE55" s="0">
         <v>0.814552</v>
@@ -15076,7 +15076,7 @@
         <v>0.853488</v>
       </c>
       <c r="BY55" s="0">
-        <v>0.822212</v>
+        <v>0.810666</v>
       </c>
       <c r="BZ55" s="0">
         <v>1.028553</v>
@@ -15165,7 +15165,7 @@
         <v>0.647436</v>
       </c>
       <c r="S56" s="0">
-        <v>0.938809</v>
+        <v>0.938884</v>
       </c>
       <c r="T56" s="0">
         <v>0.491282</v>
@@ -15198,7 +15198,7 @@
         <v>0.90465</v>
       </c>
       <c r="AD56" s="0">
-        <v>0.901104</v>
+        <v>0.90111</v>
       </c>
       <c r="AE56" s="0">
         <v>0.823719</v>
@@ -15339,7 +15339,7 @@
         <v>0.855366</v>
       </c>
       <c r="BY56" s="0">
-        <v>0.825757</v>
+        <v>0.814191</v>
       </c>
       <c r="BZ56" s="0">
         <v>1.051847</v>
@@ -15428,7 +15428,7 @@
         <v>0.658667</v>
       </c>
       <c r="S57" s="0">
-        <v>0.962647</v>
+        <v>0.962782</v>
       </c>
       <c r="T57" s="0">
         <v>0.501831</v>
@@ -15461,7 +15461,7 @@
         <v>0.907524</v>
       </c>
       <c r="AD57" s="0">
-        <v>0.9043</v>
+        <v>0.90435</v>
       </c>
       <c r="AE57" s="0">
         <v>0.826843</v>
@@ -15602,7 +15602,7 @@
         <v>0.864663</v>
       </c>
       <c r="BY57" s="0">
-        <v>0.830805</v>
+        <v>0.819162</v>
       </c>
       <c r="BZ57" s="0">
         <v>1.065342</v>
@@ -15691,7 +15691,7 @@
         <v>0.667743</v>
       </c>
       <c r="S58" s="0">
-        <v>0.968121</v>
+        <v>0.968038</v>
       </c>
       <c r="T58" s="0">
         <v>0.519055</v>
@@ -15724,7 +15724,7 @@
         <v>0.9082</v>
       </c>
       <c r="AD58" s="0">
-        <v>0.909595</v>
+        <v>0.909787</v>
       </c>
       <c r="AE58" s="0">
         <v>0.833056</v>
@@ -15865,7 +15865,7 @@
         <v>0.874329</v>
       </c>
       <c r="BY58" s="0">
-        <v>0.826878</v>
+        <v>0.815265</v>
       </c>
       <c r="BZ58" s="0">
         <v>1.08637</v>
@@ -15954,7 +15954,7 @@
         <v>0.667769</v>
       </c>
       <c r="S59" s="0">
-        <v>0.975026</v>
+        <v>0.974798</v>
       </c>
       <c r="T59" s="0">
         <v>0.532394</v>
@@ -15987,7 +15987,7 @@
         <v>0.909526</v>
       </c>
       <c r="AD59" s="0">
-        <v>0.914424</v>
+        <v>0.91444</v>
       </c>
       <c r="AE59" s="0">
         <v>0.83705</v>
@@ -16128,7 +16128,7 @@
         <v>0.871746</v>
       </c>
       <c r="BY59" s="0">
-        <v>0.826739</v>
+        <v>0.815191</v>
       </c>
       <c r="BZ59" s="0">
         <v>1.09201</v>
@@ -16217,7 +16217,7 @@
         <v>0.67543</v>
       </c>
       <c r="S60" s="0">
-        <v>0.990907</v>
+        <v>0.991119</v>
       </c>
       <c r="T60" s="0">
         <v>0.550156</v>
@@ -16250,7 +16250,7 @@
         <v>0.913788</v>
       </c>
       <c r="AD60" s="0">
-        <v>0.919526</v>
+        <v>0.919416</v>
       </c>
       <c r="AE60" s="0">
         <v>0.849003</v>
@@ -16391,7 +16391,7 @@
         <v>0.878515</v>
       </c>
       <c r="BY60" s="0">
-        <v>0.830412</v>
+        <v>0.818723</v>
       </c>
       <c r="BZ60" s="0">
         <v>1.093359</v>
@@ -16480,7 +16480,7 @@
         <v>0.681151</v>
       </c>
       <c r="S61" s="0">
-        <v>1.019192</v>
+        <v>1.019274</v>
       </c>
       <c r="T61" s="0">
         <v>0.573352</v>
@@ -16513,7 +16513,7 @@
         <v>0.916913</v>
       </c>
       <c r="AD61" s="0">
-        <v>0.922072</v>
+        <v>0.922171</v>
       </c>
       <c r="AE61" s="0">
         <v>0.846578</v>
@@ -16654,7 +16654,7 @@
         <v>0.877492</v>
       </c>
       <c r="BY61" s="0">
-        <v>0.834979</v>
+        <v>0.823264</v>
       </c>
       <c r="BZ61" s="0">
         <v>1.121952</v>
@@ -16743,7 +16743,7 @@
         <v>0.686683</v>
       </c>
       <c r="S62" s="0">
-        <v>1.014085</v>
+        <v>1.014015</v>
       </c>
       <c r="T62" s="0">
         <v>0.595562</v>
@@ -16776,7 +16776,7 @@
         <v>0.91994</v>
       </c>
       <c r="AD62" s="0">
-        <v>0.928984</v>
+        <v>0.929158</v>
       </c>
       <c r="AE62" s="0">
         <v>0.853272</v>
@@ -16917,7 +16917,7 @@
         <v>0.882403</v>
       </c>
       <c r="BY62" s="0">
-        <v>0.839742</v>
+        <v>0.827949</v>
       </c>
       <c r="BZ62" s="0">
         <v>1.140127</v>
@@ -17006,7 +17006,7 @@
         <v>0.691445</v>
       </c>
       <c r="S63" s="0">
-        <v>1.020923</v>
+        <v>1.020764</v>
       </c>
       <c r="T63" s="0">
         <v>0.608881</v>
@@ -17039,7 +17039,7 @@
         <v>0.916668</v>
       </c>
       <c r="AD63" s="0">
-        <v>0.93281</v>
+        <v>0.932319</v>
       </c>
       <c r="AE63" s="0">
         <v>0.860436</v>
@@ -17180,7 +17180,7 @@
         <v>0.887013</v>
       </c>
       <c r="BY63" s="0">
-        <v>0.84327</v>
+        <v>0.831418</v>
       </c>
       <c r="BZ63" s="0">
         <v>1.173757</v>
@@ -17269,7 +17269,7 @@
         <v>0.699276</v>
       </c>
       <c r="S64" s="0">
-        <v>1.055378</v>
+        <v>1.055467</v>
       </c>
       <c r="T64" s="0">
         <v>0.630525</v>
@@ -17302,7 +17302,7 @@
         <v>0.918411</v>
       </c>
       <c r="AD64" s="0">
-        <v>0.936899</v>
+        <v>0.936787</v>
       </c>
       <c r="AE64" s="0">
         <v>0.868468</v>
@@ -17443,7 +17443,7 @@
         <v>0.893469</v>
       </c>
       <c r="BY64" s="0">
-        <v>0.846463</v>
+        <v>0.834639</v>
       </c>
       <c r="BZ64" s="0">
         <v>1.167858</v>
@@ -17532,7 +17532,7 @@
         <v>0.706958</v>
       </c>
       <c r="S65" s="0">
-        <v>1.07563</v>
+        <v>1.075706</v>
       </c>
       <c r="T65" s="0">
         <v>0.64717</v>
@@ -17565,7 +17565,7 @@
         <v>0.927272</v>
       </c>
       <c r="AD65" s="0">
-        <v>0.943681</v>
+        <v>0.944151</v>
       </c>
       <c r="AE65" s="0">
         <v>0.875746</v>
@@ -17706,7 +17706,7 @@
         <v>0.901754</v>
       </c>
       <c r="BY65" s="0">
-        <v>0.847073</v>
+        <v>0.835204</v>
       </c>
       <c r="BZ65" s="0">
         <v>1.169198</v>
@@ -17795,7 +17795,7 @@
         <v>0.718967</v>
       </c>
       <c r="S66" s="0">
-        <v>1.077155</v>
+        <v>1.077144</v>
       </c>
       <c r="T66" s="0">
         <v>0.658521</v>
@@ -17828,7 +17828,7 @@
         <v>0.93111</v>
       </c>
       <c r="AD66" s="0">
-        <v>0.951662</v>
+        <v>0.951805</v>
       </c>
       <c r="AE66" s="0">
         <v>0.881203</v>
@@ -17969,7 +17969,7 @@
         <v>0.910723</v>
       </c>
       <c r="BY66" s="0">
-        <v>0.853503</v>
+        <v>0.841538</v>
       </c>
       <c r="BZ66" s="0">
         <v>1.165481</v>
@@ -18058,7 +18058,7 @@
         <v>0.738561</v>
       </c>
       <c r="S67" s="0">
-        <v>1.088858</v>
+        <v>1.088647</v>
       </c>
       <c r="T67" s="0">
         <v>0.674387</v>
@@ -18091,7 +18091,7 @@
         <v>0.942548</v>
       </c>
       <c r="AD67" s="0">
-        <v>0.956747</v>
+        <v>0.956025</v>
       </c>
       <c r="AE67" s="0">
         <v>0.887242</v>
@@ -18232,7 +18232,7 @@
         <v>0.921395</v>
       </c>
       <c r="BY67" s="0">
-        <v>0.865971</v>
+        <v>0.853812</v>
       </c>
       <c r="BZ67" s="0">
         <v>1.177248</v>
@@ -18321,7 +18321,7 @@
         <v>0.748836</v>
       </c>
       <c r="S68" s="0">
-        <v>1.101416</v>
+        <v>1.101458</v>
       </c>
       <c r="T68" s="0">
         <v>0.691375</v>
@@ -18354,7 +18354,7 @@
         <v>0.944981</v>
       </c>
       <c r="AD68" s="0">
-        <v>0.961086</v>
+        <v>0.961316</v>
       </c>
       <c r="AE68" s="0">
         <v>0.889655</v>
@@ -18495,7 +18495,7 @@
         <v>0.93213</v>
       </c>
       <c r="BY68" s="0">
-        <v>0.870842</v>
+        <v>0.858684</v>
       </c>
       <c r="BZ68" s="0">
         <v>1.182352</v>
@@ -18584,7 +18584,7 @@
         <v>0.765681</v>
       </c>
       <c r="S69" s="0">
-        <v>1.11647</v>
+        <v>1.116439</v>
       </c>
       <c r="T69" s="0">
         <v>0.71703</v>
@@ -18617,7 +18617,7 @@
         <v>0.951848</v>
       </c>
       <c r="AD69" s="0">
-        <v>0.968226</v>
+        <v>0.968504</v>
       </c>
       <c r="AE69" s="0">
         <v>0.896374</v>
@@ -18758,7 +18758,7 @@
         <v>0.940614</v>
       </c>
       <c r="BY69" s="0">
-        <v>0.868029</v>
+        <v>0.855874</v>
       </c>
       <c r="BZ69" s="0">
         <v>1.193824</v>
@@ -18847,7 +18847,7 @@
         <v>0.781296</v>
       </c>
       <c r="S70" s="0">
-        <v>1.13607</v>
+        <v>1.13626</v>
       </c>
       <c r="T70" s="0">
         <v>0.725086</v>
@@ -18880,7 +18880,7 @@
         <v>0.95609</v>
       </c>
       <c r="AD70" s="0">
-        <v>0.975384</v>
+        <v>0.975483</v>
       </c>
       <c r="AE70" s="0">
         <v>0.901311</v>
@@ -19021,7 +19021,7 @@
         <v>0.949465</v>
       </c>
       <c r="BY70" s="0">
-        <v>0.881201</v>
+        <v>0.868871</v>
       </c>
       <c r="BZ70" s="0">
         <v>1.236945</v>
@@ -19110,7 +19110,7 @@
         <v>0.804407</v>
       </c>
       <c r="S71" s="0">
-        <v>1.155225</v>
+        <v>1.154985</v>
       </c>
       <c r="T71" s="0">
         <v>0.739362</v>
@@ -19143,7 +19143,7 @@
         <v>0.964899</v>
       </c>
       <c r="AD71" s="0">
-        <v>0.982669</v>
+        <v>0.982152</v>
       </c>
       <c r="AE71" s="0">
         <v>0.910369</v>
@@ -19284,7 +19284,7 @@
         <v>0.960431</v>
       </c>
       <c r="BY71" s="0">
-        <v>0.891926</v>
+        <v>0.879442</v>
       </c>
       <c r="BZ71" s="0">
         <v>1.236191</v>
@@ -19373,7 +19373,7 @@
         <v>0.821188</v>
       </c>
       <c r="S72" s="0">
-        <v>1.186429</v>
+        <v>1.186648</v>
       </c>
       <c r="T72" s="0">
         <v>0.77442</v>
@@ -19406,7 +19406,7 @@
         <v>0.979252</v>
       </c>
       <c r="AD72" s="0">
-        <v>0.987536</v>
+        <v>0.987899</v>
       </c>
       <c r="AE72" s="0">
         <v>0.913543</v>
@@ -19547,7 +19547,7 @@
         <v>0.967952</v>
       </c>
       <c r="BY72" s="0">
-        <v>0.893476</v>
+        <v>0.880909</v>
       </c>
       <c r="BZ72" s="0">
         <v>1.273822</v>
@@ -19636,7 +19636,7 @@
         <v>0.829649</v>
       </c>
       <c r="S73" s="0">
-        <v>1.220399</v>
+        <v>1.22032</v>
       </c>
       <c r="T73" s="0">
         <v>0.800221</v>
@@ -19669,7 +19669,7 @@
         <v>0.987005</v>
       </c>
       <c r="AD73" s="0">
-        <v>0.989485</v>
+        <v>0.990038</v>
       </c>
       <c r="AE73" s="0">
         <v>0.922916</v>
@@ -19810,7 +19810,7 @@
         <v>0.982157</v>
       </c>
       <c r="BY73" s="0">
-        <v>0.9019</v>
+        <v>0.889266</v>
       </c>
       <c r="BZ73" s="0">
         <v>1.286563</v>
@@ -19899,7 +19899,7 @@
         <v>0.822458</v>
       </c>
       <c r="S74" s="0">
-        <v>1.217519</v>
+        <v>1.217618</v>
       </c>
       <c r="T74" s="0">
         <v>0.815527</v>
@@ -19932,7 +19932,7 @@
         <v>0.981564</v>
       </c>
       <c r="AD74" s="0">
-        <v>0.993884</v>
+        <v>0.993646</v>
       </c>
       <c r="AE74" s="0">
         <v>0.929429</v>
@@ -20073,7 +20073,7 @@
         <v>0.996958</v>
       </c>
       <c r="BY74" s="0">
-        <v>0.916662</v>
+        <v>0.903847</v>
       </c>
       <c r="BZ74" s="0">
         <v>1.238565</v>
@@ -20162,7 +20162,7 @@
         <v>0.806922</v>
       </c>
       <c r="S75" s="0">
-        <v>1.214778</v>
+        <v>1.214669</v>
       </c>
       <c r="T75" s="0">
         <v>0.842883</v>
@@ -20195,7 +20195,7 @@
         <v>0.996324</v>
       </c>
       <c r="AD75" s="0">
-        <v>0.991267</v>
+        <v>0.991035</v>
       </c>
       <c r="AE75" s="0">
         <v>0.929579</v>
@@ -20336,7 +20336,7 @@
         <v>1.005803</v>
       </c>
       <c r="BY75" s="0">
-        <v>0.920458</v>
+        <v>0.907555</v>
       </c>
       <c r="BZ75" s="0">
         <v>1.245847</v>
@@ -20425,7 +20425,7 @@
         <v>0.809652</v>
       </c>
       <c r="S76" s="0">
-        <v>1.23684</v>
+        <v>1.236859</v>
       </c>
       <c r="T76" s="0">
         <v>0.845221</v>
@@ -20458,7 +20458,7 @@
         <v>0.996704</v>
       </c>
       <c r="AD76" s="0">
-        <v>0.988111</v>
+        <v>0.988276</v>
       </c>
       <c r="AE76" s="0">
         <v>0.930135</v>
@@ -20599,7 +20599,7 @@
         <v>1.009287</v>
       </c>
       <c r="BY76" s="0">
-        <v>0.921453</v>
+        <v>0.908545</v>
       </c>
       <c r="BZ76" s="0">
         <v>1.25832</v>
@@ -20688,7 +20688,7 @@
         <v>0.817828</v>
       </c>
       <c r="S77" s="0">
-        <v>1.238876</v>
+        <v>1.238818</v>
       </c>
       <c r="T77" s="0">
         <v>0.863906</v>
@@ -20721,7 +20721,7 @@
         <v>0.994711</v>
       </c>
       <c r="AD77" s="0">
-        <v>0.986906</v>
+        <v>0.987044</v>
       </c>
       <c r="AE77" s="0">
         <v>0.934989</v>
@@ -20862,7 +20862,7 @@
         <v>1.008835</v>
       </c>
       <c r="BY77" s="0">
-        <v>0.922888</v>
+        <v>0.909959</v>
       </c>
       <c r="BZ77" s="0">
         <v>1.255895</v>
@@ -20951,7 +20951,7 @@
         <v>0.835774</v>
       </c>
       <c r="S78" s="0">
-        <v>1.251976</v>
+        <v>1.252121</v>
       </c>
       <c r="T78" s="0">
         <v>0.885371</v>
@@ -20984,7 +20984,7 @@
         <v>0.998285</v>
       </c>
       <c r="AD78" s="0">
-        <v>0.991082</v>
+        <v>0.990936</v>
       </c>
       <c r="AE78" s="0">
         <v>0.937262</v>
@@ -21125,7 +21125,7 @@
         <v>1.010803</v>
       </c>
       <c r="BY78" s="0">
-        <v>0.925095</v>
+        <v>0.912141</v>
       </c>
       <c r="BZ78" s="0">
         <v>1.283351</v>
@@ -21214,7 +21214,7 @@
         <v>0.851525</v>
       </c>
       <c r="S79" s="0">
-        <v>1.259531</v>
+        <v>1.259426</v>
       </c>
       <c r="T79" s="0">
         <v>0.908502</v>
@@ -21247,7 +21247,7 @@
         <v>0.987654</v>
       </c>
       <c r="AD79" s="0">
-        <v>0.99475</v>
+        <v>0.994224</v>
       </c>
       <c r="AE79" s="0">
         <v>0.943938</v>
@@ -21388,7 +21388,7 @@
         <v>1.001725</v>
       </c>
       <c r="BY79" s="0">
-        <v>0.930849</v>
+        <v>0.917813</v>
       </c>
       <c r="BZ79" s="0">
         <v>1.297374</v>
@@ -21477,7 +21477,7 @@
         <v>0.866159</v>
       </c>
       <c r="S80" s="0">
-        <v>1.281834</v>
+        <v>1.282205</v>
       </c>
       <c r="T80" s="0">
         <v>0.908783</v>
@@ -21510,7 +21510,7 @@
         <v>0.998509</v>
       </c>
       <c r="AD80" s="0">
-        <v>0.998294</v>
+        <v>0.99869</v>
       </c>
       <c r="AE80" s="0">
         <v>0.948686</v>
@@ -21651,7 +21651,7 @@
         <v>1.00041</v>
       </c>
       <c r="BY80" s="0">
-        <v>0.927194</v>
+        <v>0.914161</v>
       </c>
       <c r="BZ80" s="0">
         <v>1.308416</v>
@@ -21740,7 +21740,7 @@
         <v>0.877875</v>
       </c>
       <c r="S81" s="0">
-        <v>1.280315</v>
+        <v>1.279786</v>
       </c>
       <c r="T81" s="0">
         <v>0.915498</v>
@@ -21773,7 +21773,7 @@
         <v>1.003101</v>
       </c>
       <c r="AD81" s="0">
-        <v>1.002302</v>
+        <v>1.002636</v>
       </c>
       <c r="AE81" s="0">
         <v>0.945442</v>
@@ -21914,7 +21914,7 @@
         <v>0.997042</v>
       </c>
       <c r="BY81" s="0">
-        <v>0.933525</v>
+        <v>0.920433</v>
       </c>
       <c r="BZ81" s="0">
         <v>1.315189</v>
@@ -22003,7 +22003,7 @@
         <v>0.900302</v>
       </c>
       <c r="S82" s="0">
-        <v>1.310795</v>
+        <v>1.311053</v>
       </c>
       <c r="T82" s="0">
         <v>0.931609</v>
@@ -22036,7 +22036,7 @@
         <v>1.010252</v>
       </c>
       <c r="AD82" s="0">
-        <v>1.004622</v>
+        <v>1.004658</v>
       </c>
       <c r="AE82" s="0">
         <v>0.951414</v>
@@ -22177,7 +22177,7 @@
         <v>0.994796</v>
       </c>
       <c r="BY82" s="0">
-        <v>0.937375</v>
+        <v>0.924219</v>
       </c>
       <c r="BZ82" s="0">
         <v>1.327761</v>
@@ -22266,7 +22266,7 @@
         <v>0.923567</v>
       </c>
       <c r="S83" s="0">
-        <v>1.335094</v>
+        <v>1.335303</v>
       </c>
       <c r="T83" s="0">
         <v>0.941867</v>
@@ -22299,7 +22299,7 @@
         <v>1.011465</v>
       </c>
       <c r="AD83" s="0">
-        <v>1.00613</v>
+        <v>1.005765</v>
       </c>
       <c r="AE83" s="0">
         <v>0.969297</v>
@@ -22440,7 +22440,7 @@
         <v>1.005935</v>
       </c>
       <c r="BY83" s="0">
-        <v>0.939678</v>
+        <v>0.926504</v>
       </c>
       <c r="BZ83" s="0">
         <v>1.355388</v>
@@ -22529,7 +22529,7 @@
         <v>0.943418</v>
       </c>
       <c r="S84" s="0">
-        <v>1.364518</v>
+        <v>1.363957</v>
       </c>
       <c r="T84" s="0">
         <v>0.948307</v>
@@ -22562,7 +22562,7 @@
         <v>1.025713</v>
       </c>
       <c r="AD84" s="0">
-        <v>1.007804</v>
+        <v>1.008097</v>
       </c>
       <c r="AE84" s="0">
         <v>0.962386</v>
@@ -22703,7 +22703,7 @@
         <v>1.006253</v>
       </c>
       <c r="BY84" s="0">
-        <v>0.942141</v>
+        <v>0.928916</v>
       </c>
       <c r="BZ84" s="0">
         <v>1.364798</v>
@@ -22792,7 +22792,7 @@
         <v>0.957718</v>
       </c>
       <c r="S85" s="0">
-        <v>1.369196</v>
+        <v>1.368611</v>
       </c>
       <c r="T85" s="0">
         <v>0.966146</v>
@@ -22825,7 +22825,7 @@
         <v>1.031275</v>
       </c>
       <c r="AD85" s="0">
-        <v>1.010273</v>
+        <v>1.010519</v>
       </c>
       <c r="AE85" s="0">
         <v>0.963929</v>
@@ -22966,7 +22966,7 @@
         <v>1.012251</v>
       </c>
       <c r="BY85" s="0">
-        <v>0.945364</v>
+        <v>0.932107</v>
       </c>
       <c r="BZ85" s="0">
         <v>1.375869</v>
@@ -23055,7 +23055,7 @@
         <v>0.957918</v>
       </c>
       <c r="S86" s="0">
-        <v>1.408224</v>
+        <v>1.409149</v>
       </c>
       <c r="T86" s="0">
         <v>0.983168</v>
@@ -23088,7 +23088,7 @@
         <v>1.03489</v>
       </c>
       <c r="AD86" s="0">
-        <v>1.013544</v>
+        <v>1.013621</v>
       </c>
       <c r="AE86" s="0">
         <v>0.970128</v>
@@ -23229,7 +23229,7 @@
         <v>1.018002</v>
       </c>
       <c r="BY86" s="0">
-        <v>0.945854</v>
+        <v>0.932583</v>
       </c>
       <c r="BZ86" s="0">
         <v>1.346346</v>
@@ -23318,7 +23318,7 @@
         <v>0.961153</v>
       </c>
       <c r="S87" s="0">
-        <v>1.408742</v>
+        <v>1.408751</v>
       </c>
       <c r="T87" s="0">
         <v>0.994531</v>
@@ -23351,7 +23351,7 @@
         <v>1.044656</v>
       </c>
       <c r="AD87" s="0">
-        <v>1.016322</v>
+        <v>1.016559</v>
       </c>
       <c r="AE87" s="0">
         <v>0.971372</v>
@@ -23492,7 +23492,7 @@
         <v>1.013698</v>
       </c>
       <c r="BY87" s="0">
-        <v>0.94688</v>
+        <v>0.933578</v>
       </c>
       <c r="BZ87" s="0">
         <v>1.360413</v>
@@ -23581,7 +23581,7 @@
         <v>0.969485</v>
       </c>
       <c r="S88" s="0">
-        <v>1.403072</v>
+        <v>1.402579</v>
       </c>
       <c r="T88" s="0">
         <v>0.994773</v>
@@ -23614,7 +23614,7 @@
         <v>1.053796</v>
       </c>
       <c r="AD88" s="0">
-        <v>1.019935</v>
+        <v>1.019997</v>
       </c>
       <c r="AE88" s="0">
         <v>0.974813</v>
@@ -23755,7 +23755,7 @@
         <v>1.016223</v>
       </c>
       <c r="BY88" s="0">
-        <v>0.954888</v>
+        <v>0.9415</v>
       </c>
       <c r="BZ88" s="0">
         <v>1.373478</v>
@@ -23844,7 +23844,7 @@
         <v>0.971128</v>
       </c>
       <c r="S89" s="0">
-        <v>1.406781</v>
+        <v>1.406287</v>
       </c>
       <c r="T89" s="0">
         <v>1.002699</v>
@@ -23877,7 +23877,7 @@
         <v>1.059377</v>
       </c>
       <c r="AD89" s="0">
-        <v>1.023029</v>
+        <v>1.022467</v>
       </c>
       <c r="AE89" s="0">
         <v>0.986833</v>
@@ -24018,7 +24018,7 @@
         <v>1.012891</v>
       </c>
       <c r="BY89" s="0">
-        <v>0.951618</v>
+        <v>0.938331</v>
       </c>
       <c r="BZ89" s="0">
         <v>1.39819</v>
@@ -24107,7 +24107,7 @@
         <v>0.975133</v>
       </c>
       <c r="S90" s="0">
-        <v>1.423777</v>
+        <v>1.424743</v>
       </c>
       <c r="T90" s="0">
         <v>1.012358</v>
@@ -24140,7 +24140,7 @@
         <v>1.067044</v>
       </c>
       <c r="AD90" s="0">
-        <v>1.025231</v>
+        <v>1.02553</v>
       </c>
       <c r="AE90" s="0">
         <v>0.992081</v>
@@ -24281,7 +24281,7 @@
         <v>1.018022</v>
       </c>
       <c r="BY90" s="0">
-        <v>0.955823</v>
+        <v>0.942487</v>
       </c>
       <c r="BZ90" s="0">
         <v>1.414578</v>
@@ -24370,7 +24370,7 @@
         <v>0.984024</v>
       </c>
       <c r="S91" s="0">
-        <v>1.428694</v>
+        <v>1.427837</v>
       </c>
       <c r="T91" s="0">
         <v>1.019635</v>
@@ -24403,7 +24403,7 @@
         <v>1.073568</v>
       </c>
       <c r="AD91" s="0">
-        <v>1.027625</v>
+        <v>1.027488</v>
       </c>
       <c r="AE91" s="0">
         <v>0.995304</v>
@@ -24544,7 +24544,7 @@
         <v>1.016287</v>
       </c>
       <c r="BY91" s="0">
-        <v>0.956906</v>
+        <v>0.943517</v>
       </c>
       <c r="BZ91" s="0">
         <v>1.400053</v>
@@ -24633,7 +24633,7 @@
         <v>0.985977</v>
       </c>
       <c r="S92" s="0">
-        <v>1.429674</v>
+        <v>1.428294</v>
       </c>
       <c r="T92" s="0">
         <v>1.039181</v>
@@ -24666,7 +24666,7 @@
         <v>1.082304</v>
       </c>
       <c r="AD92" s="0">
-        <v>1.028893</v>
+        <v>1.029039</v>
       </c>
       <c r="AE92" s="0">
         <v>0.996856</v>
@@ -24807,7 +24807,7 @@
         <v>1.023514</v>
       </c>
       <c r="BY92" s="0">
-        <v>0.959437</v>
+        <v>0.9459</v>
       </c>
       <c r="BZ92" s="0">
         <v>1.404688</v>
@@ -24896,7 +24896,7 @@
         <v>0.991476</v>
       </c>
       <c r="S93" s="0">
-        <v>1.447569</v>
+        <v>1.447337</v>
       </c>
       <c r="T93" s="0">
         <v>1.041114</v>
@@ -24929,7 +24929,7 @@
         <v>1.084611</v>
       </c>
       <c r="AD93" s="0">
-        <v>1.029402</v>
+        <v>1.029035</v>
       </c>
       <c r="AE93" s="0">
         <v>1.00408</v>
@@ -25070,7 +25070,7 @@
         <v>1.027596</v>
       </c>
       <c r="BY93" s="0">
-        <v>0.964351</v>
+        <v>0.950919</v>
       </c>
       <c r="BZ93" s="0">
         <v>1.41628</v>
@@ -25159,7 +25159,7 @@
         <v>1.000596</v>
       </c>
       <c r="S94" s="0">
-        <v>1.448495</v>
+        <v>1.450895</v>
       </c>
       <c r="T94" s="0">
         <v>1.058737</v>
@@ -25192,7 +25192,7 @@
         <v>1.091863</v>
       </c>
       <c r="AD94" s="0">
-        <v>1.0303</v>
+        <v>1.029993</v>
       </c>
       <c r="AE94" s="0">
         <v>1.003658</v>
@@ -25333,7 +25333,7 @@
         <v>1.027497</v>
       </c>
       <c r="BY94" s="0">
-        <v>0.968914</v>
+        <v>0.955424</v>
       </c>
       <c r="BZ94" s="0">
         <v>1.426272</v>
@@ -25422,7 +25422,7 @@
         <v>0.994674</v>
       </c>
       <c r="S95" s="0">
-        <v>1.457702</v>
+        <v>1.459336</v>
       </c>
       <c r="T95" s="0">
         <v>1.077319</v>
@@ -25455,7 +25455,7 @@
         <v>1.095255</v>
       </c>
       <c r="AD95" s="0">
-        <v>1.034026</v>
+        <v>1.033204</v>
       </c>
       <c r="AE95" s="0">
         <v>1.009565</v>
@@ -25596,7 +25596,7 @@
         <v>1.02938</v>
       </c>
       <c r="BY95" s="0">
-        <v>0.971773</v>
+        <v>0.958134</v>
       </c>
       <c r="BZ95" s="0">
         <v>1.423579</v>
@@ -25685,7 +25685,7 @@
         <v>0.996667</v>
       </c>
       <c r="S96" s="0">
-        <v>1.463793</v>
+        <v>1.464448</v>
       </c>
       <c r="T96" s="0">
         <v>1.103027</v>
@@ -25718,7 +25718,7 @@
         <v>1.098248</v>
       </c>
       <c r="AD96" s="0">
-        <v>1.0336</v>
+        <v>1.033064</v>
       </c>
       <c r="AE96" s="0">
         <v>1.018655</v>
@@ -25859,7 +25859,7 @@
         <v>1.031019</v>
       </c>
       <c r="BY96" s="0">
-        <v>0.977372</v>
+        <v>0.963509</v>
       </c>
       <c r="BZ96" s="0">
         <v>1.435892</v>
@@ -25948,7 +25948,7 @@
         <v>1.002836</v>
       </c>
       <c r="S97" s="0">
-        <v>1.47088</v>
+        <v>1.471289</v>
       </c>
       <c r="T97" s="0">
         <v>1.108761</v>
@@ -25981,7 +25981,7 @@
         <v>1.104216</v>
       </c>
       <c r="AD97" s="0">
-        <v>1.033685</v>
+        <v>1.033994</v>
       </c>
       <c r="AE97" s="0">
         <v>1.021187</v>
@@ -26122,7 +26122,7 @@
         <v>1.033679</v>
       </c>
       <c r="BY97" s="0">
-        <v>0.981587</v>
+        <v>0.968053</v>
       </c>
       <c r="BZ97" s="0">
         <v>1.430435</v>
@@ -26211,7 +26211,7 @@
         <v>1.002605</v>
       </c>
       <c r="S98" s="0">
-        <v>1.481495</v>
+        <v>1.478833</v>
       </c>
       <c r="T98" s="0">
         <v>1.111086</v>
@@ -26244,7 +26244,7 @@
         <v>1.107995</v>
       </c>
       <c r="AD98" s="0">
-        <v>1.036557</v>
+        <v>1.039432</v>
       </c>
       <c r="AE98" s="0">
         <v>1.016314</v>
@@ -26385,7 +26385,7 @@
         <v>1.031626</v>
       </c>
       <c r="BY98" s="0">
-        <v>0.985775</v>
+        <v>0.97212</v>
       </c>
       <c r="BZ98" s="0">
         <v>1.429605</v>
@@ -26474,7 +26474,7 @@
         <v>0.999075</v>
       </c>
       <c r="S99" s="0">
-        <v>1.467501</v>
+        <v>1.468469</v>
       </c>
       <c r="T99" s="0">
         <v>1.128046</v>
@@ -26507,7 +26507,7 @@
         <v>1.115817</v>
       </c>
       <c r="AD99" s="0">
-        <v>1.039107</v>
+        <v>1.043124</v>
       </c>
       <c r="AE99" s="0">
         <v>1.016964</v>
@@ -26648,7 +26648,7 @@
         <v>1.037092</v>
       </c>
       <c r="BY99" s="0">
-        <v>0.995749</v>
+        <v>0.981867</v>
       </c>
       <c r="BZ99" s="0">
         <v>1.429559</v>
@@ -26737,7 +26737,7 @@
         <v>1.002594</v>
       </c>
       <c r="S100" s="0">
-        <v>1.493682</v>
+        <v>1.49372</v>
       </c>
       <c r="T100" s="0">
         <v>1.12383</v>
@@ -26770,7 +26770,7 @@
         <v>1.116435</v>
       </c>
       <c r="AD100" s="0">
-        <v>1.038626</v>
+        <v>1.044443</v>
       </c>
       <c r="AE100" s="0">
         <v>1.027057</v>
@@ -26911,7 +26911,7 @@
         <v>1.040369</v>
       </c>
       <c r="BY100" s="0">
-        <v>0.998948</v>
+        <v>0.984909</v>
       </c>
       <c r="BZ100" s="0">
         <v>1.436133</v>
@@ -27000,7 +27000,7 @@
         <v>1.000367</v>
       </c>
       <c r="S101" s="0">
-        <v>1.514707</v>
+        <v>1.514513</v>
       </c>
       <c r="T101" s="0">
         <v>1.129237</v>
@@ -27033,7 +27033,7 @@
         <v>1.122846</v>
       </c>
       <c r="AD101" s="0">
-        <v>1.041458</v>
+        <v>1.047374</v>
       </c>
       <c r="AE101" s="0">
         <v>1.023629</v>
@@ -27174,7 +27174,7 @@
         <v>1.039948</v>
       </c>
       <c r="BY101" s="0">
-        <v>1.000642</v>
+        <v>0.98687</v>
       </c>
       <c r="BZ101" s="0">
         <v>1.44561</v>
@@ -27263,7 +27263,7 @@
         <v>0.999436</v>
       </c>
       <c r="S102" s="0">
-        <v>1.54131</v>
+        <v>1.540521</v>
       </c>
       <c r="T102" s="0">
         <v>1.136373</v>
@@ -27296,7 +27296,7 @@
         <v>1.125109</v>
       </c>
       <c r="AD102" s="0">
-        <v>1.045039</v>
+        <v>1.050041</v>
       </c>
       <c r="AE102" s="0">
         <v>1.020521</v>
@@ -27437,7 +27437,7 @@
         <v>1.041456</v>
       </c>
       <c r="BY102" s="0">
-        <v>1.003468</v>
+        <v>0.989305</v>
       </c>
       <c r="BZ102" s="0">
         <v>1.443346</v>
@@ -27526,7 +27526,7 @@
         <v>1.002202</v>
       </c>
       <c r="S103" s="0">
-        <v>1.554069</v>
+        <v>1.554411</v>
       </c>
       <c r="T103" s="0">
         <v>1.137097</v>
@@ -27559,7 +27559,7 @@
         <v>1.121441</v>
       </c>
       <c r="AD103" s="0">
-        <v>1.048738</v>
+        <v>1.050251</v>
       </c>
       <c r="AE103" s="0">
         <v>1.029833</v>
@@ -27700,7 +27700,7 @@
         <v>1.046305</v>
       </c>
       <c r="BY103" s="0">
-        <v>1.00686</v>
+        <v>0.993071</v>
       </c>
       <c r="BZ103" s="0">
         <v>1.446238</v>
@@ -27789,7 +27789,7 @@
         <v>1.007239</v>
       </c>
       <c r="S104" s="0">
-        <v>1.581968</v>
+        <v>1.58389</v>
       </c>
       <c r="T104" s="0">
         <v>1.160095</v>
@@ -27822,7 +27822,7 @@
         <v>1.128778</v>
       </c>
       <c r="AD104" s="0">
-        <v>1.047584</v>
+        <v>1.048685</v>
       </c>
       <c r="AE104" s="0">
         <v>1.039455</v>
@@ -27963,7 +27963,7 @@
         <v>1.042381</v>
       </c>
       <c r="BY104" s="0">
-        <v>1.008216</v>
+        <v>0.994937</v>
       </c>
       <c r="BZ104" s="0">
         <v>1.462619</v>
@@ -28052,7 +28052,7 @@
         <v>1.011134</v>
       </c>
       <c r="S105" s="0">
-        <v>1.599908</v>
+        <v>1.597696</v>
       </c>
       <c r="T105" s="0">
         <v>1.159637</v>
@@ -28085,7 +28085,7 @@
         <v>1.131239</v>
       </c>
       <c r="AD105" s="0">
-        <v>1.049571</v>
+        <v>1.050036</v>
       </c>
       <c r="AE105" s="0">
         <v>1.040735</v>
@@ -28226,7 +28226,7 @@
         <v>1.047205</v>
       </c>
       <c r="BY105" s="0">
-        <v>1.015017</v>
+        <v>1.000877</v>
       </c>
       <c r="BZ105" s="0">
         <v>1.472103</v>
@@ -28315,7 +28315,7 @@
         <v>1.02558</v>
       </c>
       <c r="S106" s="0">
-        <v>1.633941</v>
+        <v>1.63389</v>
       </c>
       <c r="T106" s="0">
         <v>1.171823</v>
@@ -28348,7 +28348,7 @@
         <v>1.133445</v>
       </c>
       <c r="AD106" s="0">
-        <v>1.051932</v>
+        <v>1.05247</v>
       </c>
       <c r="AE106" s="0">
         <v>1.048971</v>
@@ -28489,7 +28489,7 @@
         <v>1.054048</v>
       </c>
       <c r="BY106" s="0">
-        <v>1.026245</v>
+        <v>1.012512</v>
       </c>
       <c r="BZ106" s="0">
         <v>1.47682</v>
@@ -28577,8 +28577,8 @@
       <c r="R107" s="0">
         <v>1.047518</v>
       </c>
-      <c r="S107" s="0" t="s">
-        <v>88</v>
+      <c r="S107" s="0">
+        <v>1.648234</v>
       </c>
       <c r="T107" s="0" t="s">
         <v>88</v>
@@ -28611,7 +28611,7 @@
         <v>88</v>
       </c>
       <c r="AD107" s="0">
-        <v>1.055078</v>
+        <v>1.054237</v>
       </c>
       <c r="AE107" s="0">
         <v>1.054777</v>
@@ -28751,8 +28751,8 @@
       <c r="BX107" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="BY107" s="0" t="s">
-        <v>88</v>
+      <c r="BY107" s="0">
+        <v>1.016528</v>
       </c>
       <c r="BZ107" s="0">
         <v>1.494817</v>

</xml_diff>